<commit_message>
Fix tecnologia errors and fix coordinates
</commit_message>
<xml_diff>
--- a/arquivos/id_tecnologia_facilidades.xlsx
+++ b/arquivos/id_tecnologia_facilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F257064\Documents\Codes\atualizacao nfv automatico\NEW_NFV\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B7582B-FFD6-42FE-8F37-1FECBAE2C2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED27A31-9049-481E-87A2-0B0BCAB95F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="61">
   <si>
     <t>FACILIDADE</t>
   </si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t>RADIO IP</t>
-  </si>
-  <si>
-    <t>FO GPON_RESID ETH PV</t>
   </si>
   <si>
     <t>BANDA KA</t>
@@ -542,7 +539,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,10 +586,10 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2">
         <v>8</v>
@@ -615,7 +612,7 @@
         <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G3">
         <v>8</v>
@@ -638,7 +635,7 @@
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4">
         <v>8</v>
@@ -661,7 +658,7 @@
         <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G5">
         <v>8</v>
@@ -684,7 +681,7 @@
         <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G6">
         <v>8</v>
@@ -707,7 +704,7 @@
         <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7">
         <v>8</v>
@@ -727,10 +724,10 @@
         <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G8">
         <v>8</v>
@@ -750,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -773,7 +770,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10">
         <v>8</v>
@@ -796,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11">
         <v>8</v>
@@ -819,7 +816,7 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G12">
         <v>8</v>
@@ -842,7 +839,7 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13">
         <v>8</v>
@@ -865,7 +862,7 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G14">
         <v>8</v>
@@ -888,7 +885,7 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G15">
         <v>8</v>
@@ -911,7 +908,7 @@
         <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G16">
         <v>8</v>
@@ -934,7 +931,7 @@
         <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G17">
         <v>8</v>
@@ -957,7 +954,7 @@
         <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G18">
         <v>8</v>
@@ -980,7 +977,7 @@
         <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G19">
         <v>8</v>
@@ -997,10 +994,10 @@
         <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G20">
         <v>8</v>
@@ -1017,10 +1014,10 @@
         <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G21">
         <v>8</v>
@@ -1043,7 +1040,7 @@
         <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G22">
         <v>8</v>
@@ -1066,7 +1063,7 @@
         <v>45</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G23">
         <v>8</v>
@@ -1083,7 +1080,7 @@
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1097,7 +1094,7 @@
         <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1114,7 +1111,7 @@
         <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G26">
         <v>8</v>

</xml_diff>